<commit_message>
added omicwas and toast to methods list
</commit_message>
<xml_diff>
--- a/methods-list.xlsx
+++ b/methods-list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tb13101/Desktop/projects/post-doc/cell-specifc-effects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tb13101/Desktop/projects/post-doc/cell-specific-effects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C78837-0050-4049-BCBD-3AD6BF7ED45F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBB1679-6756-3041-ACAA-6D23EBF8FA80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15440" xr2:uid="{1F620509-F48A-EE4D-9795-B8FCA0045929}"/>
+    <workbookView xWindow="780" yWindow="880" windowWidth="27640" windowHeight="15440" xr2:uid="{1F620509-F48A-EE4D-9795-B8FCA0045929}"/>
   </bookViews>
   <sheets>
     <sheet name="cell-specific-dnam" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
   <si>
     <t>name</t>
   </si>
@@ -130,6 +130,30 @@
   </si>
   <si>
     <t>see running-notes.md</t>
+  </si>
+  <si>
+    <t>omicwas</t>
+  </si>
+  <si>
+    <t>Nonlinear ridge regression improves cell-type-specific differential expression analysis</t>
+  </si>
+  <si>
+    <t>Fumihiko Takeuchi</t>
+  </si>
+  <si>
+    <t>Fumihiko Takeuchi [fumihiko@takeuchi.name]</t>
+  </si>
+  <si>
+    <t>TOAST</t>
+  </si>
+  <si>
+    <t>TOAST: improving reference-free cell composition estimation by cross-cell type differential analysis</t>
+  </si>
+  <si>
+    <t>Ziyi Li</t>
+  </si>
+  <si>
+    <t>Hao Wu [hao.wu@emory.edu]</t>
   </si>
 </sst>
 </file>
@@ -500,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D84906D4-29F5-F944-86AB-AEB80A5FA741}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -669,7 +693,50 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="1"/>
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="2">
+        <v>33752591</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9">
+        <v>31484546</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
small updates to plots
</commit_message>
<xml_diff>
--- a/methods-list.xlsx
+++ b/methods-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tb13101/Desktop/projects/post-doc/cell-specific-effects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBB1679-6756-3041-ACAA-6D23EBF8FA80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4EF8CF1-BAE0-EE46-B916-3749DE093BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="880" windowWidth="27640" windowHeight="15440" xr2:uid="{1F620509-F48A-EE4D-9795-B8FCA0045929}"/>
   </bookViews>
@@ -527,7 +527,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>